<commit_message>
Update calendar feed with 3rd entry
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulpallesen/Documents/Calendar-feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54581393-AE2F-ED4D-90E0-A2D4FF940C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB6E786-4678-504A-BDD9-8507680D109E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{DD08DFD7-F757-6F4F-853E-B722FD167EA9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Unique ID</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Transparent</t>
+  </si>
+  <si>
+    <t>TEST/EVENT</t>
+  </si>
+  <si>
+    <t>MYMY</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
   </si>
 </sst>
 </file>
@@ -158,10 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824B196F-4EAC-5C42-918D-6B09AB48F696}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,6 +642,36 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45884</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1">
+        <v>45885</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>